<commit_message>
Update menu items and add gitignore file
</commit_message>
<xml_diff>
--- a/WeeklySoir.xlsx
+++ b/WeeklySoir.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nathan.boga\Documents\__Insta-Joliot__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A44415A-3FD5-4009-B074-FE2916CB21F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD9A432F-B07D-4F76-ACA7-1DD083B081F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
   <si>
     <t>Date</t>
   </si>
@@ -84,30 +84,6 @@
     <t xml:space="preserve">Trop de légumes au romanesco </t>
   </si>
   <si>
-    <t xml:space="preserve">Feuilleté thon tomate </t>
-  </si>
-  <si>
-    <t>Guacamole fait maison</t>
-  </si>
-  <si>
-    <t>Salade de pâtes bio au surimi</t>
-  </si>
-  <si>
-    <t>Rougail saucisse</t>
-  </si>
-  <si>
-    <t>Dos de colin</t>
-  </si>
-  <si>
-    <t>Riz bio au curry</t>
-  </si>
-  <si>
-    <t>Duo de haricots</t>
-  </si>
-  <si>
-    <t>Tartelette meringuée</t>
-  </si>
-  <si>
     <t>Entree 4</t>
   </si>
   <si>
@@ -175,6 +151,21 @@
   </si>
   <si>
     <t>Carottes bio vichy</t>
+  </si>
+  <si>
+    <t>Salade de pomme de terre</t>
+  </si>
+  <si>
+    <t>Crépinette de porc BBC</t>
+  </si>
+  <si>
+    <t>Boulettes pois chiches</t>
+  </si>
+  <si>
+    <t>Lentilles</t>
+  </si>
+  <si>
+    <t>Carottes braisées</t>
   </si>
 </sst>
 </file>
@@ -533,8 +524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,7 +558,7 @@
         <v>9</v>
       </c>
       <c r="F1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="G1" t="s">
         <v>10</v>
@@ -613,28 +604,19 @@
         <v>45545</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="G3" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="H3" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="I3" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="J3" t="s">
-        <v>25</v>
-      </c>
-      <c r="K3" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -645,28 +627,28 @@
         <v>45546</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="F4" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="G4" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="H4" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="I4" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="J4" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -677,31 +659,31 @@
         <v>45547</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
         <v>28</v>
       </c>
-      <c r="D5" t="s">
-        <v>36</v>
-      </c>
       <c r="E5" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F5" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="G5" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="H5" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="I5" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="J5" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="K5" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -712,28 +694,28 @@
         <v>45548</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="E6" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="F6" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="G6" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="H6" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="I6" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="J6" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>